<commit_message>
Fixed Excel test data and login validation failures
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Valid" sheetId="1" r:id="rId5"/>
-    <sheet state="visible" name="invalid" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="VALID" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="INVALID" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>

</xml_diff>

<commit_message>
Fixed DataProvider issue and updated DB verification test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="VALID" sheetId="1" r:id="rId5"/>
     <sheet state="visible" name="INVALID" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="EmployeeDetails" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -20,13 +21,28 @@
     <t>password</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>admin123</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>dheeraj913</t>
+  </si>
+  <si>
+    <t>@Dksharmais1908</t>
+  </si>
+  <si>
+    <t>admindemo</t>
+  </si>
+  <si>
+    <t>emp_id</t>
+  </si>
+  <si>
+    <t>emp_name</t>
+  </si>
+  <si>
+    <t>Dheeraj</t>
+  </si>
+  <si>
+    <t>Ajay</t>
+  </si>
+  <si>
+    <t>Ravi</t>
   </si>
 </sst>
 </file>
@@ -80,6 +96,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -341,4 +361,51 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated on 28th jan
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Dheeraj</t>
-  </si>
-  <si>
-    <t>Ajay</t>
-  </si>
-  <si>
-    <t>Ravi</t>
   </si>
 </sst>
 </file>
@@ -389,22 +383,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>